<commit_message>
Update to CR excel template
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@3828 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-10.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4665" windowWidth="19440" windowHeight="5460" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="4725" windowWidth="19440" windowHeight="5400" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="4" state="hidden" r:id="rId1"/>
@@ -1343,6 +1343,15 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF9EC4D8"/>
+      <color rgb="FFFF6600"/>
+      <color rgb="FF384332"/>
+      <color rgb="FF1F497D"/>
+      <color rgb="FFCCA8EA"/>
+      <color rgb="FFB3E5FC"/>
+      <color rgb="FF33CCFF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1638,7 +1647,7 @@
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="0"/>
@@ -1653,28 +1662,27 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="0">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="E8B7FF"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="CD9EF4"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000"/>
-            </a:gradFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw dist="35921" dir="2700000" algn="br">
-                <a:srgbClr val="000000"/>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF6600"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1743,11 +1751,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="80387072"/>
-        <c:axId val="80544512"/>
+        <c:axId val="29579904"/>
+        <c:axId val="29602176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80387072"/>
+        <c:axId val="29579904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,7 +1783,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80544512"/>
+        <c:crossAx val="29602176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1783,7 +1791,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80544512"/>
+        <c:axId val="29602176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,7 +1819,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80387072"/>
+        <c:crossAx val="29579904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1826,16 +1834,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.8647482014388489"/>
-          <c:y val="0.36503067484662577"/>
-          <c:w val="0.1223021582733813"/>
-          <c:h val="0.32515337423312884"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -1973,7 +1972,7 @@
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1988,27 +1987,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="0">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:srgbClr val="B1F1FF"/>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:srgbClr val="89CAE2"/>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000"/>
-            </a:gradFill>
-            <a:ln w="25400">
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw dist="35921" dir="2700000" algn="br">
-                <a:srgbClr val="000000"/>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
@@ -2016,16 +1994,8 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="br">
-                  <a:srgbClr val="000000"/>
-                </a:outerShdw>
-              </a:effectLst>
             </c:spPr>
           </c:dPt>
           <c:dPt>
@@ -2036,14 +2006,6 @@
               <a:solidFill>
                 <a:srgbClr val="FF6600"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="br">
-                  <a:srgbClr val="000000"/>
-                </a:outerShdw>
-              </a:effectLst>
             </c:spPr>
           </c:dPt>
           <c:dPt>
@@ -2052,16 +2014,8 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="93C5D8"/>
+                <a:srgbClr val="9EC4D8"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="br">
-                  <a:srgbClr val="000000"/>
-                </a:outerShdw>
-              </a:effectLst>
             </c:spPr>
           </c:dPt>
           <c:cat>
@@ -2110,12 +2064,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="80587008"/>
-        <c:axId val="80588800"/>
+        <c:axId val="29968256"/>
+        <c:axId val="29969792"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="80587008"/>
+        <c:axId val="29968256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2143,7 +2097,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80588800"/>
+        <c:crossAx val="29969792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2151,7 +2105,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80588800"/>
+        <c:axId val="29969792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2179,7 +2133,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80587008"/>
+        <c:crossAx val="29968256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2256,6 +2210,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2338,7 +2293,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:srgbClr val="33CCFF"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -2348,7 +2303,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="B3E5FC"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -2358,7 +2313,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:srgbClr val="CCA8EA"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -2368,7 +2323,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:srgbClr val="1F497D"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -2424,12 +2379,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="80755712"/>
-        <c:axId val="80761600"/>
+        <c:axId val="30008448"/>
+        <c:axId val="30009984"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="80755712"/>
+        <c:axId val="30008448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2457,7 +2412,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80761600"/>
+        <c:crossAx val="30009984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2465,7 +2420,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80761600"/>
+        <c:axId val="30009984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2493,7 +2448,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80755712"/>
+        <c:crossAx val="30008448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2576,6 +2531,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2609,7 +2565,7 @@
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2625,6 +2581,26 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF6600"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:txPr>
               <a:bodyPr/>
@@ -2687,12 +2663,12 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="80806272"/>
-        <c:axId val="80808960"/>
+        <c:axId val="29732864"/>
+        <c:axId val="29735552"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="80806272"/>
+        <c:axId val="29732864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2715,7 +2691,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80808960"/>
+        <c:crossAx val="29735552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2723,7 +2699,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80808960"/>
+        <c:axId val="29735552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2734,35 +2710,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80806272"/>
+        <c:crossAx val="29732864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.72251058111899435"/>
-          <c:y val="9.6529233058466113E-2"/>
-          <c:w val="0.2418118552301585"/>
-          <c:h val="3.2090352060029761E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -6449,7 +6401,7 @@
       <c r="P114" s="155"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9C2B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="M43:P43"/>
     <mergeCell ref="M88:P88"/>
@@ -7795,7 +7747,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9C2B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
@@ -8464,7 +8416,7 @@
       <c r="I45" s="37"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9C2B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="3">
     <mergeCell ref="H28:I29"/>
     <mergeCell ref="F28:G29"/>
@@ -10031,7 +9983,7 @@
       <c r="Q60" s="37"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9C2B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
@@ -48149,7 +48101,7 @@
       <c r="R2000" s="124"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9C2B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
@@ -48370,7 +48322,7 @@
       <c r="C28"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="9C2B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Updated consolidated report template
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@3829 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-10.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-10.xlsx
@@ -1433,6 +1433,18 @@
               </a:solidFill>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:txPr>
               <a:bodyPr/>
@@ -1751,11 +1763,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="29579904"/>
-        <c:axId val="29602176"/>
+        <c:axId val="29064576"/>
+        <c:axId val="28906624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="29579904"/>
+        <c:axId val="29064576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1783,7 +1795,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29602176"/>
+        <c:crossAx val="28906624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1791,7 +1803,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29602176"/>
+        <c:axId val="28906624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1819,7 +1831,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="29579904"/>
+        <c:crossAx val="29064576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1834,7 +1846,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -2064,12 +2075,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="29968256"/>
-        <c:axId val="29969792"/>
+        <c:axId val="28940928"/>
+        <c:axId val="28942720"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="29968256"/>
+        <c:axId val="28940928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2097,7 +2108,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29969792"/>
+        <c:crossAx val="28942720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2105,7 +2116,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29969792"/>
+        <c:axId val="28942720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,7 +2144,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="29968256"/>
+        <c:crossAx val="28940928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2379,12 +2390,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="30008448"/>
-        <c:axId val="30009984"/>
+        <c:axId val="29112192"/>
+        <c:axId val="29113728"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="30008448"/>
+        <c:axId val="29112192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2412,7 +2423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30009984"/>
+        <c:crossAx val="29113728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2420,7 +2431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30009984"/>
+        <c:axId val="29113728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2448,7 +2459,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="30008448"/>
+        <c:crossAx val="29112192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2663,12 +2674,12 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="29732864"/>
-        <c:axId val="29735552"/>
+        <c:axId val="29129344"/>
+        <c:axId val="29157632"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="29732864"/>
+        <c:axId val="29129344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2691,7 +2702,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29735552"/>
+        <c:crossAx val="29157632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2699,7 +2710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29735552"/>
+        <c:axId val="29157632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2710,7 +2721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="29732864"/>
+        <c:crossAx val="29129344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>